<commit_message>
added some nice new test models
</commit_message>
<xml_diff>
--- a/Tests/integrationTests/ARE startup/Test_cases_ARE_startup.xlsx
+++ b/Tests/integrationTests/ARE startup/Test_cases_ARE_startup.xlsx
@@ -175,7 +175,7 @@
     <t>ARE_START_5</t>
   </si>
   <si>
-    <t>Use model file xxx (not up 2 date with bundle_descriptors)
+    <t>Use damaged model file xxx (not up 2 date with bundle_descriptors)
 Start Are with start_debug.bat (start_debug.sh)</t>
   </si>
 </sst>
@@ -544,7 +544,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -554,7 +554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added test cases and models for ARE startup
</commit_message>
<xml_diff>
--- a/Tests/integrationTests/ARE startup/Test_cases_ARE_startup.xlsx
+++ b/Tests/integrationTests/ARE startup/Test_cases_ARE_startup.xlsx
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Number</t>
   </si>
@@ -175,8 +175,60 @@
     <t>ARE_START_5</t>
   </si>
   <si>
-    <t>Use damaged model file xxx (not up 2 date with bundle_descriptors)
-Start Are with start_debug.bat (start_debug.sh)</t>
+    <t>Use damaged model file autostart_damaged.acs (xml-schema error)</t>
+  </si>
+  <si>
+    <t>1. Execute ARE start file</t>
+  </si>
+  <si>
+    <t>ARE start file: Are.exe - Windows only</t>
+  </si>
+  <si>
+    <t>ARE start file: start_debug.bat (start_debug.sh - Linux)</t>
+  </si>
+  <si>
+    <t>ARE start file: start.bat (start.sh - Linux)</t>
+  </si>
+  <si>
+    <t>ARE start file: Are.exe (start.sh - Linux)
+model file: ARE startup/autostart_damaged.acs</t>
+  </si>
+  <si>
+    <t>ARE start file: Are.exe (start.sh - Linux)
+ARE startup/Ergo-Kopf-Musik-einfach_v2.5.acs</t>
+  </si>
+  <si>
+    <t>Use old model file Ergo-Kopf-Musik-einfach_v2.5.acs (not up 2 date with bundle_descriptors of used plugins)</t>
+  </si>
+  <si>
+    <t>1. Backup original model file models/autostart.xml
+2. Copy model file to models/autostart.xml
+3.Execute ARE start file
+4. Restore original model file</t>
+  </si>
+  <si>
+    <t>Note: If no error dialogs are shown in the ARE gui, ensure to set the following property in the fie 'areProperties':
+showErrorDialogs=1</t>
+  </si>
+  <si>
+    <t>ARE_START_6</t>
+  </si>
+  <si>
+    <t>Use old model file GamepadMouse.acs (without plugging in Gamepad)</t>
+  </si>
+  <si>
+    <t>ARE start file: Are.exe (start.sh - Linux)
+ARE startup/GamepadMouse.acs</t>
+  </si>
+  <si>
+    <t>1. Backup original model file models/autostart.xml
+2. Copy model file to models/autostart.xml
+3. DO NOT plug in Gamepad
+4.Execute ARE start file
+5. Restore original model file</t>
+  </si>
+  <si>
+    <t>ARE should start with the model running and  show up informative error message</t>
   </si>
 </sst>
 </file>
@@ -544,7 +596,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -554,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,9 +632,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
@@ -613,10 +668,14 @@
         <v>10</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E7" s="5" t="s">
         <v>11</v>
       </c>
@@ -627,10 +686,14 @@
         <v>12</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E8" s="5" t="s">
         <v>11</v>
       </c>
@@ -641,10 +704,14 @@
         <v>13</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E9" s="5" t="s">
         <v>11</v>
       </c>
@@ -657,8 +724,12 @@
       <c r="B10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="C10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E10" s="5" t="s">
         <v>18</v>
       </c>
@@ -668,18 +739,36 @@
       <c r="A11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="101.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="A12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="140.44999999999999" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>